<commit_message>
Done changes in Excel and Done Code Modifications
</commit_message>
<xml_diff>
--- a/src/test/resource/TestData/testDataSheet.xlsx
+++ b/src/test/resource/TestData/testDataSheet.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="11325" windowHeight="3525" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="11325" windowHeight="3525" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Register" sheetId="3" r:id="rId3"/>
     <sheet name="Customer" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="InvalidLoginDetails" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>TC_ID</t>
   </si>
@@ -50,12 +50,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Test1234</t>
-  </si>
-  <si>
     <t>password_invalid</t>
   </si>
   <si>
@@ -180,6 +174,39 @@
   </si>
   <si>
     <t>sjdhkjsdhfqwuqwyeiu</t>
+  </si>
+  <si>
+    <t>manjunath1234</t>
+  </si>
+  <si>
+    <t>nitin111</t>
+  </si>
+  <si>
+    <t>nitin11212</t>
+  </si>
+  <si>
+    <t>autoenroll1</t>
+  </si>
+  <si>
+    <t>jayeshbulk1</t>
+  </si>
+  <si>
+    <t>santhosh123</t>
+  </si>
+  <si>
+    <t>FavText</t>
+  </si>
+  <si>
+    <t>pawankalyan</t>
+  </si>
+  <si>
+    <t>rancheran</t>
+  </si>
+  <si>
+    <t>chinajivi</t>
+  </si>
+  <si>
+    <t>pawanKalyan</t>
   </si>
 </sst>
 </file>
@@ -592,19 +619,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,21 +642,97 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" display="test@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -661,58 +765,58 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>27</v>
-      </c>
-      <c r="R1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -720,13 +824,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>12345</v>
@@ -735,43 +839,43 @@
         <v>9900224430</v>
       </c>
       <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
-        <v>38</v>
       </c>
       <c r="N2">
         <v>2005</v>
       </c>
       <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" t="s">
         <v>39</v>
-      </c>
-      <c r="P2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>41</v>
       </c>
       <c r="R2">
         <v>6</v>
       </c>
       <c r="S2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -783,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -797,22 +901,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -820,10 +924,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <v>9880306309</v>
@@ -832,10 +936,10 @@
         <v>87789789</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -848,12 +952,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>